<commit_message>
Implement WinSCP Sync and vscode Tasks
</commit_message>
<xml_diff>
--- a/zeitaufzeichnung.xlsx
+++ b/zeitaufzeichnung.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA4155E-4E30-4751-8F2F-C9E3DE69E61F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A8BD05-2CF3-4A91-96EB-78D75EED9E00}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1800" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Stunden</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>AWS Env - Config AnsibleHost/Smoketest</t>
+  </si>
+  <si>
+    <t>16:30 - 18:00</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <dimension ref="A2:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +431,7 @@
       </c>
       <c r="C2">
         <f>SUM(A5:A58)</f>
-        <v>21.75</v>
+        <v>23.25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,12 +533,14 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>1.5</v>
+      </c>
       <c r="B11" s="2">
         <v>43503</v>
       </c>
-      <c r="C11" s="4">
-        <v>0.6875</v>
+      <c r="C11" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
@@ -543,8 +548,12 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="B12" s="2">
+        <v>43503</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
work on slides, exercise 1 ansible_facts
</commit_message>
<xml_diff>
--- a/zeitaufzeichnung.xlsx
+++ b/zeitaufzeichnung.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A8BD05-2CF3-4A91-96EB-78D75EED9E00}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8761B061-1B06-42E6-BE47-0811817E2C4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1800" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Stunden</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Zeitraum</t>
-  </si>
-  <si>
-    <t>20:00-23:0</t>
   </si>
   <si>
     <t>Tasks</t>
@@ -58,9 +55,6 @@
     <t>Übersicht</t>
   </si>
   <si>
-    <t>15:30 - 16:00, 19:30-21:15</t>
-  </si>
-  <si>
     <t>Präsentation</t>
   </si>
   <si>
@@ -70,12 +64,6 @@
     <t>20:00 - 24:00</t>
   </si>
   <si>
-    <t>19:00-24:00</t>
-  </si>
-  <si>
-    <t>19:00-20:00, 22:30-01:00</t>
-  </si>
-  <si>
     <t>AWS Environment</t>
   </si>
   <si>
@@ -83,6 +71,39 @@
   </si>
   <si>
     <t>16:30 - 18:00</t>
+  </si>
+  <si>
+    <t>20:30 - 23:30</t>
+  </si>
+  <si>
+    <t>WinSCP Syncing, vscode Task Sequences</t>
+  </si>
+  <si>
+    <t>22:30 - 01:00</t>
+  </si>
+  <si>
+    <t>19:30 - 21:15</t>
+  </si>
+  <si>
+    <t>19:00 - 24:00</t>
+  </si>
+  <si>
+    <t>19:00 - 20:00</t>
+  </si>
+  <si>
+    <t>20:00 - 23:0</t>
+  </si>
+  <si>
+    <t>15:30 - 16:00</t>
+  </si>
+  <si>
+    <t>20:15 - 21:15</t>
+  </si>
+  <si>
+    <t>19:30 - 00:00</t>
+  </si>
+  <si>
+    <t>Präsentation/Übungs 1 - ansible_facts/aws fixes</t>
   </si>
 </sst>
 </file>
@@ -412,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D35"/>
+  <dimension ref="A2:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,11 +448,11 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <f>SUM(A5:A58)</f>
-        <v>23.25</v>
+        <f>SUM(A5:A60)</f>
+        <v>31.75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -445,7 +466,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -456,10 +477,10 @@
         <v>43488</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -470,38 +491,38 @@
         <v>43489</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>2.25</v>
+        <v>0.5</v>
       </c>
       <c r="B7" s="2">
         <v>43491</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>4</v>
+        <v>1.75</v>
       </c>
       <c r="B8" s="2">
-        <v>43496</v>
+        <v>43491</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -509,76 +530,112 @@
         <v>4</v>
       </c>
       <c r="B9" s="2">
-        <v>43499</v>
+        <v>43496</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2">
-        <v>43502</v>
+        <v>43499</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>43502</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B12" s="2">
+        <v>43502</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>1.5</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B13" s="2">
         <v>43503</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2">
+      <c r="C13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2">
         <v>43503</v>
       </c>
-      <c r="C12" s="4">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43504</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="A16" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B16" s="2">
+        <v>43507</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -694,6 +751,18 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
slides - debug,vars, inventory vars, directory layouts
</commit_message>
<xml_diff>
--- a/zeitaufzeichnung.xlsx
+++ b/zeitaufzeichnung.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8761B061-1B06-42E6-BE47-0811817E2C4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59562996-8AEE-461C-B115-6042D81B61DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1800" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31245" yWindow="4620" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Stunden</t>
   </si>
@@ -103,7 +103,19 @@
     <t>19:30 - 00:00</t>
   </si>
   <si>
-    <t>Präsentation/Übungs 1 - ansible_facts/aws fixes</t>
+    <t>20:00 - 23:30</t>
+  </si>
+  <si>
+    <t>Präsentation/Übung 2 - simple playbook</t>
+  </si>
+  <si>
+    <t>Präsentation/Übung 1 - ansible_facts/aws fixes</t>
+  </si>
+  <si>
+    <t>Präsentation - Vars / Inventory Layouts / group_vars,host_vars</t>
+  </si>
+  <si>
+    <t>21:00 - 23:00</t>
   </si>
 </sst>
 </file>
@@ -436,7 +448,7 @@
   <dimension ref="A2:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +464,11 @@
       </c>
       <c r="C2">
         <f>SUM(A5:A60)</f>
-        <v>31.75</v>
+        <v>37.25</v>
+      </c>
+      <c r="D2">
+        <f>C2*20</f>
+        <v>745</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -634,20 +650,36 @@
         <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43509</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="A18" s="1">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2">
+        <v>43510</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>

</xml_diff>

<commit_message>
Minor Changes and slides for templates and loops
</commit_message>
<xml_diff>
--- a/zeitaufzeichnung.xlsx
+++ b/zeitaufzeichnung.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37A9783-CD76-479E-98DB-D89F411B2EA6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D42702-6FC7-4F2B-B717-A9BA6AAA241D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31245" yWindow="4620" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1920" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Stunden</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>20:00 - 23:00</t>
+  </si>
+  <si>
+    <t>Präsentation - Ansible Templates</t>
+  </si>
+  <si>
+    <t>13:30 - 15:30</t>
+  </si>
+  <si>
+    <t>10:30 - 11:45</t>
+  </si>
+  <si>
+    <t>Präsentation - Ansible Loops</t>
   </si>
 </sst>
 </file>
@@ -453,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,11 +482,11 @@
       </c>
       <c r="C2">
         <f>SUM(A5:A60)</f>
-        <v>40.25</v>
+        <v>43.5</v>
       </c>
       <c r="D2">
         <f>C2*20</f>
-        <v>805</v>
+        <v>870</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,16 +714,32 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="A20" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="B20" s="2">
+        <v>43530</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2">
+        <v>43530</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>

</xml_diff>

<commit_message>
Übung 3 fertig gestellt.
</commit_message>
<xml_diff>
--- a/zeitaufzeichnung.xlsx
+++ b/zeitaufzeichnung.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A0B257-2CC3-4989-8D37-9107554F113D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD0E347-1490-4118-A43A-85C26929F088}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1920" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Stunden</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Präsentation - Conditionals</t>
+  </si>
+  <si>
+    <t>16:30-18:00</t>
+  </si>
+  <si>
+    <t>Prästation - Übung 3</t>
   </si>
 </sst>
 </file>
@@ -472,7 +478,7 @@
   <dimension ref="A2:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,11 +494,11 @@
       </c>
       <c r="C2">
         <f>SUM(A5:A60)</f>
-        <v>44</v>
+        <v>45.5</v>
       </c>
       <c r="D2">
         <f>C2*20</f>
-        <v>880</v>
+        <v>910</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -762,10 +768,18 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="A23" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B23" s="2">
+        <v>43549</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>

</xml_diff>

<commit_message>
include_playbook, lookup, delegate, run_once, block
</commit_message>
<xml_diff>
--- a/zeitaufzeichnung.xlsx
+++ b/zeitaufzeichnung.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD0E347-1490-4118-A43A-85C26929F088}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E135BBD-5406-4D51-9FD8-71E919680B50}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1920" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19920" yWindow="5025" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Stunden</t>
   </si>
@@ -146,6 +146,21 @@
   </si>
   <si>
     <t>Prästation - Übung 3</t>
+  </si>
+  <si>
+    <t>19:00:00-20:00</t>
+  </si>
+  <si>
+    <t>Präsentation - block, delegate_to</t>
+  </si>
+  <si>
+    <t>10:00-11:30</t>
+  </si>
+  <si>
+    <t>Präs. lookup, include_tasks, include_playbook</t>
+  </si>
+  <si>
+    <t>16:16 - 17:15</t>
   </si>
 </sst>
 </file>
@@ -477,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,11 +509,11 @@
       </c>
       <c r="C2">
         <f>SUM(A5:A60)</f>
-        <v>45.5</v>
+        <v>49</v>
       </c>
       <c r="D2">
         <f>C2*20</f>
-        <v>910</v>
+        <v>980</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -782,22 +797,46 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2">
+        <v>43551</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="A25" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B25" s="2">
+        <v>43552</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2">
+        <v>43552</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>

</xml_diff>

<commit_message>
Working Hard :-) Deathline coming!
</commit_message>
<xml_diff>
--- a/zeitaufzeichnung.xlsx
+++ b/zeitaufzeichnung.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611951AA-0E4A-4E96-9965-08B285219D79}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB79DFD-98CD-4B72-B123-4E06BDDB1041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1800" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1215" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Stunden</t>
   </si>
@@ -176,6 +178,12 @@
   </si>
   <si>
     <t>Präs. galaxy, minor changes</t>
+  </si>
+  <si>
+    <t>Präs. roles, demo/workshop roles</t>
+  </si>
+  <si>
+    <t>17:00-21:30</t>
   </si>
 </sst>
 </file>
@@ -507,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,11 +532,11 @@
       </c>
       <c r="C2">
         <f>SUM(A5:A60)</f>
-        <v>53</v>
+        <v>56.5</v>
       </c>
       <c r="D2">
         <f>C2*20</f>
-        <v>1060</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,10 +904,18 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="A30" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B30" s="2">
+        <v>43844</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>

</xml_diff>

<commit_message>
Plenty of work :-)
</commit_message>
<xml_diff>
--- a/zeitaufzeichnung.xlsx
+++ b/zeitaufzeichnung.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32EEA9A-A9FD-4CCB-80D8-1231C668DE0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB574B34-5087-4AEA-8821-7D811C9ABD24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1215" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>Stunden</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>17:00-21:30</t>
+  </si>
+  <si>
+    <t>Präs. zusatz, best practice</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
   <dimension ref="A2:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,11 +535,11 @@
       </c>
       <c r="C2">
         <f>SUM(A5:A60)</f>
-        <v>56.5</v>
+        <v>62</v>
       </c>
       <c r="D2">
         <f>C2*20</f>
-        <v>1130</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -905,7 +908,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="B30" s="2">
         <v>43844</v>
@@ -918,10 +921,18 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="A31" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B31" s="2">
+        <v>43845</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>

</xml_diff>